<commit_message>
add new fileds in the model
</commit_message>
<xml_diff>
--- a/tracks.xlsx
+++ b/tracks.xlsx
@@ -507,31 +507,6 @@
       <c r="E2" t="n">
         <v>292880</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>05/14/2022</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>4vu7F6h90Br1ZtYYaqfITy</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>['711MCceyCBcFnzjGY4Q7Un']</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>383d95c22b2f7f42b125a6f2919698b3</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>05/16/2022</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -555,31 +530,6 @@
       <c r="E3" t="n">
         <v>354640</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>05/12/2022</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>5EsAeGDozof1PIH3WPXLr2</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>['7HL4id2U7FSDJtfKQHMgQx']</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>3375d943fe0a049d971dcc8be0a43f95</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>05/16/2022</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -603,31 +553,6 @@
       <c r="E4" t="n">
         <v>214853</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>05/12/2022</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>3JwFNl80WWeXPiKEjIFbqa</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>['711MCceyCBcFnzjGY4Q7Un']</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>3140e5d6301e73993e8038f41c3962ee</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>05/16/2022</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -651,31 +576,6 @@
       <c r="E5" t="n">
         <v>331266</v>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>05/12/2022</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>2Kh43m04B1UkVcpcRa1Zug</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>['2ye2Wgw4gimLv2eAKyk1NB']</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>75dcecd7d568a2310d4fc483a6766357</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>05/16/2022</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -699,31 +599,6 @@
       <c r="E6" t="n">
         <v>255493</v>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>05/12/2022</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>6mUdeDZCsExyJLMdAfDuwh</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>['711MCceyCBcFnzjGY4Q7Un']</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>ddbfaee8fa065468a412697d9991c3d0</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>05/16/2022</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -747,31 +622,6 @@
       <c r="E7" t="n">
         <v>211066</v>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>05/10/2022</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>3WNxdumkSMGMJRhEgK80qx</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>['26dSoYclwsYLMAKD3tpOr4']</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>cdc5c77b2e1a6eab3a59501013ac4a01</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>05/16/2022</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -795,31 +645,6 @@
       <c r="E8" t="n">
         <v>248413</v>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>05/10/2022</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>2ePFIvZKMe8zefATp9ofFA</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>['4tZwfgrHOc3mvqYlEYSvVi', '2RdwBSPQiwcmiDo9kixcl8', '3yDIp0kaq9EFKe07X1X2rz']</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>a8c1ec9e466bc544081ce55c9a0717d2</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>05/16/2022</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -843,31 +668,6 @@
       <c r="E9" t="n">
         <v>232160</v>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>05/10/2022</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>4T1zaLt2uHXf8qAscsSP60</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>['2Ax9wZpdlg4r2zkc3pcI8U']</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>f4009ddfc3392e5adaf202687ca6a9b3</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>05/16/2022</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -891,31 +691,6 @@
       <c r="E10" t="n">
         <v>163520</v>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>05/10/2022</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>1NdnBLYZy9ZtgzPbyxdM5E</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>['3CoaObestry7i9joSvJ2hK']</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>46323c8f371606a6b72ea82c930e7f32</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>05/16/2022</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -938,31 +713,6 @@
       </c>
       <c r="E11" t="n">
         <v>180133</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>05/10/2022</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>0ufPamcshkfTyzmIJp9Efi</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>['7jerD1mbWgyDukHAmCvdCj']</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>143746c51b5b23da61652a64734d80aa</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>05/16/2022</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>